<commit_message>
sc5 pro power on success
Change-Id: I14d3f72abe7620bdd958ca487ee833889bf277f9

Former-commit-id: 1b438ca9d56bfd380ab24e3ecaf2f9f7421230b1
</commit_message>
<xml_diff>
--- a/SC5PRO/config.xlsx
+++ b/SC5PRO/config.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="969" uniqueCount="337">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="864" uniqueCount="339">
   <si>
     <t xml:space="preserve">Pin number</t>
   </si>
@@ -3561,16 +3561,22 @@
     <t xml:space="preserve">VQPS-1.8V</t>
   </si>
   <si>
+    <t xml:space="preserve">SYS-RST-DEASSERT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SYS_RST_DEASSERT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PG-DDR-0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DDR_POWER_GOOD</t>
+  </si>
+  <si>
     <t xml:space="preserve">SYS-RST-ASSERT</t>
   </si>
   <si>
-    <t xml:space="preserve">SYS-RST-DEASSERT</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PG-DDR-0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PG-DDR-1</t>
+    <t xml:space="preserve">SYS_RST_ASSERT</t>
   </si>
 </sst>
 </file>
@@ -3837,8 +3843,8 @@
   </sheetPr>
   <dimension ref="A1:L101"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A43" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C59" activeCellId="0" sqref="C59"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A31" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F48" activeCellId="0" sqref="F48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4086,21 +4092,11 @@
       <c r="C7" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="D7" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="E7" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="F7" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="G7" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="H7" s="4" t="s">
-        <v>18</v>
-      </c>
+      <c r="D7" s="4"/>
+      <c r="E7" s="4"/>
+      <c r="F7" s="4"/>
+      <c r="G7" s="4"/>
+      <c r="H7" s="4"/>
       <c r="I7" s="3"/>
       <c r="J7" s="5"/>
       <c r="K7" s="6" t="s">
@@ -4226,21 +4222,11 @@
       <c r="C11" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="D11" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="E11" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="F11" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="G11" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="H11" s="4" t="s">
-        <v>18</v>
-      </c>
+      <c r="D11" s="4"/>
+      <c r="E11" s="4"/>
+      <c r="F11" s="4"/>
+      <c r="G11" s="4"/>
+      <c r="H11" s="4"/>
       <c r="I11" s="3"/>
       <c r="J11" s="5"/>
       <c r="K11" s="6" t="s">
@@ -4366,21 +4352,11 @@
       <c r="C15" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="D15" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="E15" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="F15" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="G15" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="H15" s="4" t="s">
-        <v>18</v>
-      </c>
+      <c r="D15" s="4"/>
+      <c r="E15" s="4"/>
+      <c r="F15" s="4"/>
+      <c r="G15" s="4"/>
+      <c r="H15" s="4"/>
       <c r="I15" s="3"/>
       <c r="J15" s="5"/>
       <c r="K15" s="6" t="s">
@@ -4530,21 +4506,11 @@
       <c r="C20" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="D20" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="E20" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="F20" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="G20" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="H20" s="4" t="s">
-        <v>18</v>
-      </c>
+      <c r="D20" s="4"/>
+      <c r="E20" s="4"/>
+      <c r="F20" s="4"/>
+      <c r="G20" s="4"/>
+      <c r="H20" s="4"/>
       <c r="I20" s="3"/>
       <c r="J20" s="5"/>
       <c r="K20" s="9" t="s">
@@ -4562,21 +4528,11 @@
       <c r="C21" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="D21" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="E21" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="F21" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="G21" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="H21" s="4" t="s">
-        <v>18</v>
-      </c>
+      <c r="D21" s="4"/>
+      <c r="E21" s="4"/>
+      <c r="F21" s="4"/>
+      <c r="G21" s="4"/>
+      <c r="H21" s="4"/>
       <c r="I21" s="3"/>
       <c r="J21" s="5"/>
       <c r="K21" s="9" t="s">
@@ -4594,21 +4550,11 @@
       <c r="C22" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="D22" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="E22" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="F22" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="G22" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="H22" s="4" t="s">
-        <v>18</v>
-      </c>
+      <c r="D22" s="4"/>
+      <c r="E22" s="4"/>
+      <c r="F22" s="4"/>
+      <c r="G22" s="4"/>
+      <c r="H22" s="4"/>
       <c r="I22" s="3"/>
       <c r="J22" s="5"/>
       <c r="K22" s="6" t="s">
@@ -4626,21 +4572,11 @@
       <c r="C23" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="D23" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="E23" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="F23" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="G23" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="H23" s="4" t="s">
-        <v>18</v>
-      </c>
+      <c r="D23" s="4"/>
+      <c r="E23" s="4"/>
+      <c r="F23" s="4"/>
+      <c r="G23" s="4"/>
+      <c r="H23" s="4"/>
       <c r="I23" s="3"/>
       <c r="J23" s="5"/>
       <c r="K23" s="6" t="s">
@@ -4796,21 +4732,11 @@
       <c r="C28" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="D28" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="E28" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="F28" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="G28" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="H28" s="4" t="s">
-        <v>18</v>
-      </c>
+      <c r="D28" s="4"/>
+      <c r="E28" s="4"/>
+      <c r="F28" s="4"/>
+      <c r="G28" s="4"/>
+      <c r="H28" s="4"/>
       <c r="I28" s="3"/>
       <c r="J28" s="5"/>
       <c r="K28" s="9" t="s">
@@ -4828,21 +4754,11 @@
       <c r="C29" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="D29" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="E29" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="F29" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="G29" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="H29" s="4" t="s">
-        <v>18</v>
-      </c>
+      <c r="D29" s="4"/>
+      <c r="E29" s="4"/>
+      <c r="F29" s="4"/>
+      <c r="G29" s="4"/>
+      <c r="H29" s="4"/>
       <c r="I29" s="3"/>
       <c r="J29" s="5"/>
       <c r="K29" s="6" t="s">
@@ -5558,21 +5474,11 @@
       <c r="C50" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="D50" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="E50" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="F50" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="G50" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="H50" s="4" t="s">
-        <v>18</v>
-      </c>
+      <c r="D50" s="4"/>
+      <c r="E50" s="4"/>
+      <c r="F50" s="4"/>
+      <c r="G50" s="4"/>
+      <c r="H50" s="4"/>
       <c r="I50" s="3"/>
       <c r="J50" s="5"/>
       <c r="K50" s="9" t="s">
@@ -5591,18 +5497,10 @@
         <v>34</v>
       </c>
       <c r="D51" s="4"/>
-      <c r="E51" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="F51" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="G51" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="H51" s="4" t="s">
-        <v>18</v>
-      </c>
+      <c r="E51" s="4"/>
+      <c r="F51" s="4"/>
+      <c r="G51" s="4"/>
+      <c r="H51" s="4"/>
       <c r="I51" s="3"/>
       <c r="J51" s="5"/>
       <c r="K51" s="6" t="s">
@@ -6359,18 +6257,10 @@
         <v>222</v>
       </c>
       <c r="D73" s="4"/>
-      <c r="E73" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="F73" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="G73" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="H73" s="4" t="s">
-        <v>18</v>
-      </c>
+      <c r="E73" s="4"/>
+      <c r="F73" s="4"/>
+      <c r="G73" s="4"/>
+      <c r="H73" s="4"/>
       <c r="I73" s="3"/>
       <c r="J73" s="5"/>
       <c r="K73" s="6" t="s">
@@ -6389,18 +6279,10 @@
         <v>34</v>
       </c>
       <c r="D74" s="4"/>
-      <c r="E74" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="F74" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="G74" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="H74" s="4" t="s">
-        <v>18</v>
-      </c>
+      <c r="E74" s="4"/>
+      <c r="F74" s="4"/>
+      <c r="G74" s="4"/>
+      <c r="H74" s="4"/>
       <c r="I74" s="3"/>
       <c r="J74" s="5"/>
       <c r="K74" s="6" t="s">
@@ -6419,18 +6301,10 @@
         <v>77</v>
       </c>
       <c r="D75" s="4"/>
-      <c r="E75" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="F75" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="G75" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="H75" s="4" t="s">
-        <v>18</v>
-      </c>
+      <c r="E75" s="4"/>
+      <c r="F75" s="4"/>
+      <c r="G75" s="4"/>
+      <c r="H75" s="4"/>
       <c r="I75" s="3"/>
       <c r="J75" s="5"/>
       <c r="K75" s="9" t="s">
@@ -6449,18 +6323,10 @@
         <v>34</v>
       </c>
       <c r="D76" s="4"/>
-      <c r="E76" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="F76" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="G76" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="H76" s="4" t="s">
-        <v>18</v>
-      </c>
+      <c r="E76" s="4"/>
+      <c r="F76" s="4"/>
+      <c r="G76" s="4"/>
+      <c r="H76" s="4"/>
       <c r="I76" s="3"/>
       <c r="J76" s="5"/>
       <c r="K76" s="6" t="s">
@@ -6479,18 +6345,10 @@
         <v>227</v>
       </c>
       <c r="D77" s="4"/>
-      <c r="E77" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="F77" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="G77" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="H77" s="4" t="s">
-        <v>18</v>
-      </c>
+      <c r="E77" s="4"/>
+      <c r="F77" s="4"/>
+      <c r="G77" s="4"/>
+      <c r="H77" s="4"/>
       <c r="I77" s="3"/>
       <c r="J77" s="5"/>
       <c r="K77" s="6" t="s">
@@ -6869,18 +6727,10 @@
         <v>46</v>
       </c>
       <c r="D88" s="4"/>
-      <c r="E88" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="F88" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="G88" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="H88" s="4" t="s">
-        <v>18</v>
-      </c>
+      <c r="E88" s="4"/>
+      <c r="F88" s="4"/>
+      <c r="G88" s="4"/>
+      <c r="H88" s="4"/>
       <c r="I88" s="3"/>
       <c r="J88" s="10"/>
       <c r="K88" s="6" t="s">
@@ -7115,18 +6965,10 @@
         <v>277</v>
       </c>
       <c r="D95" s="4"/>
-      <c r="E95" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="F95" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="G95" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="H95" s="4" t="s">
-        <v>18</v>
-      </c>
+      <c r="E95" s="4"/>
+      <c r="F95" s="4"/>
+      <c r="G95" s="4"/>
+      <c r="H95" s="4"/>
       <c r="I95" s="3"/>
       <c r="J95" s="10" t="s">
         <v>70</v>
@@ -7283,18 +7125,10 @@
         <v>77</v>
       </c>
       <c r="D100" s="4"/>
-      <c r="E100" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="F100" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="G100" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="H100" s="4" t="s">
-        <v>18</v>
-      </c>
+      <c r="E100" s="4"/>
+      <c r="F100" s="4"/>
+      <c r="G100" s="4"/>
+      <c r="H100" s="4"/>
       <c r="I100" s="3"/>
       <c r="J100" s="10"/>
       <c r="K100" s="9" t="s">
@@ -7313,18 +7147,10 @@
         <v>34</v>
       </c>
       <c r="D101" s="4"/>
-      <c r="E101" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="F101" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="G101" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="H101" s="4" t="s">
-        <v>18</v>
-      </c>
+      <c r="E101" s="4"/>
+      <c r="F101" s="4"/>
+      <c r="G101" s="4"/>
+      <c r="H101" s="4"/>
       <c r="I101" s="3"/>
       <c r="J101" s="10"/>
       <c r="K101" s="6" t="s">
@@ -7370,10 +7196,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H19"/>
+  <dimension ref="A1:H18"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C12" activeCellId="0" sqref="C12"/>
+      <selection pane="topLeft" activeCell="C18" activeCellId="0" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -7781,112 +7607,68 @@
         <v>333</v>
       </c>
       <c r="B16" s="12" t="s">
-        <v>241</v>
-      </c>
-      <c r="C16" s="12" t="s">
-        <v>198</v>
-      </c>
-      <c r="D16" s="12" t="s">
-        <v>109</v>
-      </c>
-      <c r="E16" s="12" t="s">
-        <v>118</v>
-      </c>
+        <v>334</v>
+      </c>
+      <c r="C16" s="12"/>
+      <c r="D16" s="12"/>
+      <c r="E16" s="12"/>
       <c r="F16" s="12" t="s">
-        <v>302</v>
+        <v>310</v>
       </c>
       <c r="G16" s="12" t="n">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="H16" s="12" t="n">
-        <v>29600</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="12" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="B17" s="12" t="s">
-        <v>229</v>
-      </c>
-      <c r="C17" s="12" t="s">
-        <v>256</v>
-      </c>
-      <c r="D17" s="12" t="s">
-        <v>115</v>
-      </c>
-      <c r="E17" s="12" t="s">
-        <v>142</v>
-      </c>
+        <v>336</v>
+      </c>
+      <c r="C17" s="12"/>
+      <c r="D17" s="12"/>
+      <c r="E17" s="12"/>
       <c r="F17" s="12" t="s">
-        <v>302</v>
+        <v>310</v>
       </c>
       <c r="G17" s="12" t="n">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="H17" s="12" t="n">
-        <v>0</v>
+        <v>30000</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="12" t="s">
-        <v>335</v>
+        <v>337</v>
       </c>
       <c r="B18" s="12" t="s">
-        <v>250</v>
-      </c>
-      <c r="C18" s="12" t="s">
-        <v>260</v>
-      </c>
-      <c r="D18" s="12" t="s">
-        <v>106</v>
-      </c>
-      <c r="E18" s="12" t="s">
-        <v>54</v>
-      </c>
+        <v>338</v>
+      </c>
+      <c r="C18" s="12"/>
+      <c r="D18" s="12"/>
+      <c r="E18" s="12"/>
       <c r="F18" s="12" t="s">
-        <v>302</v>
+        <v>310</v>
       </c>
       <c r="G18" s="12" t="n">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="H18" s="12" t="n">
-        <v>600</v>
-      </c>
-    </row>
-    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="12" t="s">
-        <v>336</v>
-      </c>
-      <c r="B19" s="12" t="s">
-        <v>289</v>
-      </c>
-      <c r="C19" s="12" t="s">
-        <v>124</v>
-      </c>
-      <c r="D19" s="12" t="s">
-        <v>83</v>
-      </c>
-      <c r="E19" s="12" t="s">
-        <v>97</v>
-      </c>
-      <c r="F19" s="12" t="s">
-        <v>302</v>
-      </c>
-      <c r="G19" s="12" t="n">
-        <v>100</v>
-      </c>
-      <c r="H19" s="12" t="n">
-        <v>600</v>
+        <v>30000</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="F2:F19" type="list">
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="F2:F18" type="list">
       <formula1>"ENABLE,FUNCTION"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="G2:G19" type="none">
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="G2:G18" type="none">
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>

</xml_diff>

<commit_message>
sc5pro: refactor for production release
Change-Id: Ibb0542e88fdb9c2c40e5b198f1d5b17a43e5b018

Former-commit-id: 72a78e27bcb6e0395106c41627d2848a6a53c416
</commit_message>
<xml_diff>
--- a/SC5PRO/config.xlsx
+++ b/SC5PRO/config.xlsx
@@ -5,11 +5,12 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="pin" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="power" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="adc2ver" sheetId="3" state="visible" r:id="rId4"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -21,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="864" uniqueCount="339">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="870" uniqueCount="345">
   <si>
     <t xml:space="preserve">Pin number</t>
   </si>
@@ -3577,6 +3578,24 @@
   </si>
   <si>
     <t xml:space="preserve">SYS_RST_ASSERT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">version number</t>
+  </si>
+  <si>
+    <t xml:space="preserve">r1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">r2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">voltage</t>
+  </si>
+  <si>
+    <t xml:space="preserve">limit-low</t>
+  </si>
+  <si>
+    <t xml:space="preserve">adc value</t>
   </si>
 </sst>
 </file>
@@ -3699,7 +3718,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="18">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -3762,6 +3781,14 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="4" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -3843,8 +3870,8 @@
   </sheetPr>
   <dimension ref="A1:L101"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A31" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F48" activeCellId="0" sqref="F48"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A22" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C45" activeCellId="0" sqref="C45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -7198,7 +7225,7 @@
   </sheetPr>
   <dimension ref="A1:H18"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C18" activeCellId="0" sqref="C18"/>
     </sheetView>
   </sheetViews>
@@ -7681,4 +7708,144 @@
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:F5"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F3" activeCellId="0" sqref="F3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="1" style="0" width="8.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="17.68"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="6" style="0" width="8.67"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>339</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>340</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>341</v>
+      </c>
+      <c r="D1" s="0" t="s">
+        <v>342</v>
+      </c>
+      <c r="E1" s="0" t="s">
+        <v>343</v>
+      </c>
+      <c r="F1" s="0" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="16" t="n">
+        <v>0</v>
+      </c>
+      <c r="B2" s="17" t="n">
+        <v>4700</v>
+      </c>
+      <c r="C2" s="17" t="n">
+        <v>4700</v>
+      </c>
+      <c r="D2" s="17" t="n">
+        <f aca="false">1.8*C2/(C2+B2)</f>
+        <v>0.9</v>
+      </c>
+      <c r="E2" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2" s="0" t="n">
+        <f aca="false">E2*4096/1.8</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="16" t="n">
+        <v>1</v>
+      </c>
+      <c r="B3" s="17" t="n">
+        <v>4700</v>
+      </c>
+      <c r="C3" s="17" t="n">
+        <v>10000</v>
+      </c>
+      <c r="D3" s="17" t="n">
+        <f aca="false">1.8*C3/(C3+B3)</f>
+        <v>1.22448979591837</v>
+      </c>
+      <c r="E3" s="0" t="n">
+        <f aca="false">D3-(D3-D2)/2</f>
+        <v>1.06224489795919</v>
+      </c>
+      <c r="F3" s="0" t="n">
+        <f aca="false">E3*4096/1.8</f>
+        <v>2417.19727891157</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="16" t="n">
+        <v>2</v>
+      </c>
+      <c r="B4" s="17" t="n">
+        <v>4700</v>
+      </c>
+      <c r="C4" s="17" t="n">
+        <v>20000</v>
+      </c>
+      <c r="D4" s="17" t="n">
+        <f aca="false">1.8*C4/(C4+B4)</f>
+        <v>1.45748987854251</v>
+      </c>
+      <c r="E4" s="0" t="n">
+        <f aca="false">D4-(D4-D3)/2</f>
+        <v>1.34098983723044</v>
+      </c>
+      <c r="F4" s="0" t="n">
+        <f aca="false">E4*4096/1.8</f>
+        <v>3051.49687405327</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="16" t="n">
+        <v>3</v>
+      </c>
+      <c r="B5" s="17" t="n">
+        <v>4700</v>
+      </c>
+      <c r="C5" s="17" t="n">
+        <v>47000</v>
+      </c>
+      <c r="D5" s="17" t="n">
+        <f aca="false">1.8*C5/(C5+B5)</f>
+        <v>1.63636363636364</v>
+      </c>
+      <c r="E5" s="0" t="n">
+        <f aca="false">D5-(D5-D4)/2</f>
+        <v>1.54692675745308</v>
+      </c>
+      <c r="F5" s="0" t="n">
+        <f aca="false">E5*4096/1.8</f>
+        <v>3520.11777695989</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>